<commit_message>
Added direct SAGA Quenching Plots. Updated LFs with new MW analogs.
</commit_message>
<xml_diff>
--- a/DataFiles/AdditionalData/LumFunc.xlsx
+++ b/DataFiles/AdditionalData/LumFunc.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jdvannest/Pynbody/MilkyWayAnalogs/AdditionalData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jdvannest/Pynbody/MilkyWayAnalogs/DataFiles/AdditionalData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75A6E710-640F-3C49-90E6-E52422DFCA49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6335A791-DF7F-BA48-A767-E9BD80D52910}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="500" windowWidth="28040" windowHeight="16060" xr2:uid="{8F2EF17A-7CC1-7F40-8CBF-12BD1FB2A0CD}"/>
+    <workbookView xWindow="340" yWindow="500" windowWidth="28040" windowHeight="15960" xr2:uid="{8F2EF17A-7CC1-7F40-8CBF-12BD1FB2A0CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="wpd_datasets__3" localSheetId="0">Sheet1!$M$1:$P$11</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -30,8 +33,23 @@
 </workbook>
 </file>
 
+<file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{FAB391E5-886A-F446-9972-5D849AF31C98}" name="wpd_datasets (3)" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr codePage="10000" sourceFile="/Users/jdvannest/Downloads/wpd_datasets (3).csv" comma="1">
+      <textFields count="4">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+</connections>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
   <si>
     <t>MW</t>
   </si>
@@ -55,6 +73,12 @@
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>NGC4258</t>
+  </si>
+  <si>
+    <t>NGC4631</t>
   </si>
 </sst>
 </file>
@@ -108,6 +132,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="wpd_datasets (3)" connectionId="1" xr16:uid="{7EF4998F-940F-9F49-9A9B-8844FCDA6B07}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -407,10 +435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1B602CC-14B4-C346-9CE4-14547158A37D}">
-  <dimension ref="A1:L33"/>
+  <dimension ref="A1:P33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -418,10 +446,15 @@
     <col min="1" max="1" width="20" style="1" customWidth="1"/>
     <col min="2" max="2" width="10.83203125" style="1"/>
     <col min="3" max="3" width="22.1640625" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="1"/>
+    <col min="4" max="12" width="10.83203125" style="1"/>
+    <col min="13" max="13" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -440,8 +473,14 @@
       <c r="K1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>-18.303217131103501</v>
       </c>
@@ -478,8 +517,20 @@
       <c r="L2" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>-18.303217131103501</v>
       </c>
@@ -516,8 +567,20 @@
       <c r="L3" s="1">
         <v>1.00705681083056</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M3" s="1">
+        <v>-20.928427534010702</v>
+      </c>
+      <c r="N3" s="1">
+        <v>0.99827686625497203</v>
+      </c>
+      <c r="O3" s="1">
+        <v>-20.2448234448165</v>
+      </c>
+      <c r="P3" s="1">
+        <v>0.99850609175770999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>-18.302171151587299</v>
       </c>
@@ -554,8 +617,20 @@
       <c r="L4" s="1">
         <v>2.0077603224220399</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M4" s="1">
+        <v>-14.326310452583501</v>
+      </c>
+      <c r="N4" s="1">
+        <v>2.9783333588174199</v>
+      </c>
+      <c r="O4" s="1">
+        <v>-18.8644138699485</v>
+      </c>
+      <c r="P4" s="1">
+        <v>1.9927097222925501</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>-17.001304285433299</v>
       </c>
@@ -592,8 +667,20 @@
       <c r="L5" s="1">
         <v>3.0005172532380202</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M5" s="1">
+        <v>-12.938960891248399</v>
+      </c>
+      <c r="N5" s="1">
+        <v>3.9829083134689802</v>
+      </c>
+      <c r="O5" s="1">
+        <v>-16.7281163912841</v>
+      </c>
+      <c r="P5" s="1">
+        <v>3.0000166045424201</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>-17.0002583059171</v>
       </c>
@@ -630,8 +717,20 @@
       <c r="L6" s="1">
         <v>4.00109989492484</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M6" s="1">
+        <v>-11.5335210985227</v>
+      </c>
+      <c r="N6" s="1">
+        <v>4.9803238053782799</v>
+      </c>
+      <c r="O6" s="1">
+        <v>-13.724150960127799</v>
+      </c>
+      <c r="P6" s="1">
+        <v>4.0033132083253697</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>-13.7009582830628</v>
       </c>
@@ -668,8 +767,20 @@
       <c r="L7" s="1">
         <v>5.01522921396844</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M7" s="1">
+        <v>-10.737072829374601</v>
+      </c>
+      <c r="N7" s="1">
+        <v>7.0453599279374099</v>
+      </c>
+      <c r="O7" s="1">
+        <v>-13.602778307915599</v>
+      </c>
+      <c r="P7" s="1">
+        <v>5.00368019170672</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>-13.6999208074451</v>
       </c>
@@ -700,8 +811,14 @@
       <c r="L8" s="1">
         <v>6.0151214641302504</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O8" s="1">
+        <v>-12.8719360441691</v>
+      </c>
+      <c r="P8" s="1">
+        <v>6.0082084910268501</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>-13.599370711510501</v>
       </c>
@@ -732,8 +849,14 @@
       <c r="L9" s="1">
         <v>7.0208306216276002</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O9" s="1">
+        <v>-10.635486849689499</v>
+      </c>
+      <c r="P9" s="1">
+        <v>7.00784056674732</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>-13.6046091129902</v>
       </c>
@@ -764,8 +887,14 @@
       <c r="L10" s="1">
         <v>8.0177442092736406</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O10" s="1">
+        <v>-10.4123277292942</v>
+      </c>
+      <c r="P10" s="1">
+        <v>9.0220426825113993</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>-12.1969077699057</v>
       </c>
@@ -796,8 +925,14 @@
       <c r="L11" s="1">
         <v>9.0176016132911094</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O11" s="1">
+        <v>-9.5987916712451309</v>
+      </c>
+      <c r="P11" s="1">
+        <v>10.0214932825539</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>-12.195853286490999</v>
       </c>
@@ -823,7 +958,7 @@
         <v>10.017969072600399</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>-11.297195307974</v>
       </c>
@@ -849,7 +984,7 @@
         <v>11.026788693117</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>-11.2961493284577</v>
       </c>
@@ -875,7 +1010,7 @@
         <v>12.025022527161999</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>-10.994499040653899</v>
       </c>
@@ -901,7 +1036,7 @@
         <v>13.0318555456191</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="C16" s="1">
         <v>-12.797061903066099</v>
       </c>

</xml_diff>